<commit_message>
añadidas mas estadisticas. Queda grafico evolucion de ppms
</commit_message>
<xml_diff>
--- a/docs/PROCEDIMIENTOS DATASET.xlsx
+++ b/docs/PROCEDIMIENTOS DATASET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CURSOS\Python\mini_projects\MecanOdei\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3685C313-2956-46A5-988C-1B540D3A06D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A7A13D-E4CA-4A18-AED9-F01A83977784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>tipo_emergencia</t>
   </si>
@@ -177,13 +177,7 @@
     <t>1 FUV + 1 AEA + 4 TT + (1BFP)</t>
   </si>
   <si>
-    <t>2 O 3</t>
-  </si>
-  <si>
     <t>1 FUV + 1 AEA + 6 TT + (1BFP)</t>
-  </si>
-  <si>
-    <t>3 O 4</t>
   </si>
   <si>
     <t>RAT</t>
@@ -305,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -317,9 +311,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -608,54 +599,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="3" customWidth="1"/>
     <col min="4" max="4" width="48.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="3"/>
+    <col min="10" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -778,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -994,7 +984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1005,7 +995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1022,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1042,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1062,7 +1052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1111,7 +1101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1134,7 +1124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -1157,7 +1147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -1183,7 +1173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1212,7 +1202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1229,7 +1219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -1249,7 +1239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -1269,7 +1259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
@@ -1311,11 +1301,8 @@
       <c r="I31" s="3">
         <v>4</v>
       </c>
-      <c r="J31" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
@@ -1337,11 +1324,8 @@
       <c r="I32" s="3">
         <v>5</v>
       </c>
-      <c r="J32" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
@@ -1366,11 +1350,8 @@
       <c r="I33" s="3">
         <v>8</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
@@ -1378,7 +1359,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>47</v>
@@ -1398,22 +1379,19 @@
       <c r="I34" s="3">
         <v>12</v>
       </c>
-      <c r="J34" s="4" t="s">
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G35" s="3">
         <v>1</v>
@@ -1425,18 +1403,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="3">
-        <v>2</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G36" s="3">
         <v>1</v>
@@ -1448,18 +1426,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" s="3">
         <v>3</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
@@ -1474,18 +1452,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B38" s="3">
         <v>4</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -1503,18 +1481,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="G39" s="3">
         <v>1</v>
@@ -1526,15 +1504,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" s="3">
         <v>2</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
@@ -1549,55 +1527,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
+    </row>
+    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="3">
-        <v>2</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="C43" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="I43" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="4">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="4">
-        <v>2</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="H44" s="4">
         <v>1</v>
       </c>
@@ -1605,15 +1583,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>65</v>
+    <row r="45" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B45" s="4">
         <v>3</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H45" s="4">
         <v>1</v>
@@ -1622,32 +1600,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="I46" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I46" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H47" s="4">
         <v>1</v>

</xml_diff>